<commit_message>
Update final hardcoded sample questions and answers
</commit_message>
<xml_diff>
--- a/Sample Questions Demo Py.xlsx
+++ b/Sample Questions Demo Py.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LuisBernal\Documents\Luis Bernal - Pingahla\PDQA\OpenAI Assistant API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4266A44-F452-4FF0-8BB7-FACD326D0471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B6BBEB-E4D9-4373-B851-20CF8CCB36C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{32A1D3D8-7DB6-4891-B9DE-DFC0363A4AA3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Question</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Answer</t>
   </si>
   <si>
-    <t>which columns has the least number of errors</t>
-  </si>
-  <si>
     <t>what is the total number of error hits?</t>
   </si>
   <si>
@@ -59,48 +56,47 @@
     <t>which alogorithm has the most error hits?It looks like the dataset includes columns for Table Name, Rule Type, Metric Name, Column Name, Error Hits, and Batch ID. To identify which algorithm has the most error hits, we need to focus on the "Rule Type" and "Error Hits" columns. Let's aggregate the error hits by algorithm and find out which one has the most errors.The algorithm with the most error hits is "Accuracy," which has a total of 18,467 error hits.</t>
   </si>
   <si>
-    <t>list the top five columns with table with the highest number of error hits.</t>
-  </si>
-  <si>
-    <t>list the top five columns with table with the highest number of error hits.The dataset contains the following columns: 
-- Table Name
-- Rule Type
-- Metric Name
-- Column Name
-- Error Hits
-- Batch ID
-To find the top five columns with the highest number of error hits, we will filter and aggregate by the `Column Name` and `Error Hits` fields. Let's proceed with this analysis.The top five columns with the highest number of error hits are:
-1. **Table: DIMCUSTOMER, Column: TITLE** - 18,467 error hits
-2. **Table: DIMCUSTOMER, Column: ADDRESSLINE2** - 18,236 error hits
-3. **Table: DIMCUSTOMER, Column: TOTALCHILDREN** - 2,862 error hits
-4. **Table: -, Column: -** - 227 error hits
-5. **Table: DIMCUSTOMER, Column: CUSTOMERKEY** - 75 error hits
-It appears that most of the high error hits are concentrated in the `DIMCUSTOMER` table. If you have any specific questions or need further analysis, please let me know!</t>
-  </si>
-  <si>
-    <t>which columns has the least number of errors?Let's start by loading the CSV file and inspecting its contents to understand the structure of the data. After that, we can analyze the data to identify which columns have the least number of errors.
-I'll begin loading the data from the uploaded CSV file.The data includes the following columns: 
+    <t>test</t>
+  </si>
+  <si>
+    <t>testans</t>
+  </si>
+  <si>
+    <t>which column has the least number of errors?It looks like the dataset contains the following columns:
 - `Table Name`
 - `Rule Type`
 - `Metric Name`
 - `Column Name`
 - `Error Hits`
 - `Batch ID`
-To determine which columns have the least number of errors, we need to analyze the `Error Hits` column grouped by the `Column Name`.
-Let's proceed to summarize this data by `Column Name` to find the column with the least number of errors.There are multiple columns that have the least number of errors, which in this case is zero (`0` error hits). The columns with zero error hits are:
-- ADDRESS
-- ADDRESSLINE1
-- BIRTHDATE
-- CARRIERTRACKINGNUMBER
-- CITY
-- ... and many more (total of 64 columns).
-If you need any further analysis or details on specific columns, please let me know!</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>testans</t>
+Our task is to find the column (from `Column Name`) which has the least number of `Error Hits`. Let's filter the data and identify that column.The column with the least number of errors that is not zero is `ADDRESSLINE2` in the `DIMCUSTOMER` table. It has 33 error hits.</t>
+  </si>
+  <si>
+    <t>which columns has the least number of errors?</t>
+  </si>
+  <si>
+    <t>list the top five columns with table with the highest number of error hits</t>
+  </si>
+  <si>
+    <t>list the top five columns with table with the highest number of error hits.The data consists of the following columns:
+- `Table Name`
+- `Rule Type`
+- `Metric Name`
+- `Column Name`
+- `Error Hits`
+- `Batch ID`
+list the top five columns with table with the highest number of error hits.The top five columns and table pairs with the highest number of error hits are:
+1. **Table:** DIMCUSTOMER, **Column:** TITLE, **Error Hits:** 18,467
+2. **Table:** DIMCUSTOMER, **Column:** ADDRESSLINE2, **Error Hits:** 18,236
+3. **Table:** DIMCUSTOMER, **Column:** TOTALCHILDREN, **Error Hits:** 2,862
+4. **Table:** -, **Column:** -, **Error Hits:** 227
+5. **Table:** DIMCUSTOMER, **Column:** CUSTOMERKEY, **Error Hits:** 75</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>testans2</t>
   </si>
 </sst>
 </file>
@@ -143,15 +139,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D0E801D-3B5A-4D74-AA12-D7071EC1AB50}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -508,42 +502,50 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>